<commit_message>
add optimizers study results
</commit_message>
<xml_diff>
--- a/paper/comparison/655-optimizers-medium_iterations.xlsx
+++ b/paper/comparison/655-optimizers-medium_iterations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,42 +441,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>gdpa-pd-lr3-d1.5-b10.9-b20.999-e0.1-g0.9</t>
+          <t>gdpa-pd</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>gdpa-pd-lr3-d1.5-b10.9-b20.999-e0.1-g1.5</t>
+          <t>gdpa-adam</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>gdpa-pd-lr3-d1.5-b10.9-b20.999-e0.1-g5</t>
+          <t>gdpa-noise</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>gdpa-adam-lr3-d1.5-b10.9-b20.999-e0.1</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>gdpa-noise-lr3-d1.5-g0.9</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>gdpa-noise-lr3-d1.5-g1.5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>gdpa-noise-lr3-d1.5-g5</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>gdpa-direct-lr3-d1.5</t>
+          <t>gdpa-direct</t>
         </is>
       </c>
     </row>
@@ -499,18 +479,6 @@
       <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -531,18 +499,6 @@
       <c r="F3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -563,18 +519,6 @@
       <c r="F4" t="n">
         <v>1.04</v>
       </c>
-      <c r="G4" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1.04</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -595,18 +539,6 @@
       <c r="F5" t="n">
         <v>1.06</v>
       </c>
-      <c r="G5" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1.06</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -627,18 +559,6 @@
       <c r="F6" t="n">
         <v>1.06</v>
       </c>
-      <c r="G6" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1.06</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -648,7 +568,7 @@
         <v>1.1</v>
       </c>
       <c r="C7" t="n">
-        <v>1.12</v>
+        <v>1.08</v>
       </c>
       <c r="D7" t="n">
         <v>1.08</v>
@@ -657,18 +577,6 @@
         <v>1.08</v>
       </c>
       <c r="F7" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="J7" t="n">
         <v>1.1</v>
       </c>
     </row>
@@ -680,27 +588,15 @@
         <v>1.16</v>
       </c>
       <c r="C8" t="n">
-        <v>1.24</v>
+        <v>1.18</v>
       </c>
       <c r="D8" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E8" t="n">
         <v>1.16</v>
       </c>
-      <c r="E8" t="n">
-        <v>1.14</v>
-      </c>
       <c r="F8" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1.16</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="J8" t="n">
         <v>1.14</v>
       </c>
     </row>
@@ -712,27 +608,15 @@
         <v>1.2</v>
       </c>
       <c r="C9" t="n">
-        <v>1.26</v>
+        <v>1.2</v>
       </c>
       <c r="D9" t="n">
-        <v>1.18</v>
+        <v>1.22</v>
       </c>
       <c r="E9" t="n">
-        <v>1.22</v>
+        <v>1.2</v>
       </c>
       <c r="F9" t="n">
-        <v>1.22</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="J9" t="n">
         <v>1.2</v>
       </c>
     </row>
@@ -744,27 +628,15 @@
         <v>1.4</v>
       </c>
       <c r="C10" t="n">
-        <v>1.84</v>
+        <v>1.44</v>
       </c>
       <c r="D10" t="n">
         <v>1.4</v>
       </c>
       <c r="E10" t="n">
-        <v>1.4</v>
+        <v>1.42</v>
       </c>
       <c r="F10" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1.54</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="J10" t="n">
         <v>1.42</v>
       </c>
     </row>
@@ -776,27 +648,15 @@
         <v>1.76</v>
       </c>
       <c r="C11" t="n">
-        <v>2.52</v>
+        <v>1.86</v>
       </c>
       <c r="D11" t="n">
-        <v>2.24</v>
+        <v>1.68</v>
       </c>
       <c r="E11" t="n">
         <v>1.68</v>
       </c>
       <c r="F11" t="n">
-        <v>1.68</v>
-      </c>
-      <c r="G11" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1.76</v>
-      </c>
-      <c r="J11" t="n">
         <v>1.76</v>
       </c>
     </row>
@@ -808,27 +668,15 @@
         <v>3.78</v>
       </c>
       <c r="C12" t="n">
-        <v>3.4</v>
+        <v>2.56</v>
       </c>
       <c r="D12" t="n">
-        <v>2.1</v>
+        <v>2.02</v>
       </c>
       <c r="E12" t="n">
-        <v>2.02</v>
+        <v>3.36</v>
       </c>
       <c r="F12" t="n">
-        <v>2.02</v>
-      </c>
-      <c r="G12" t="n">
-        <v>3.72</v>
-      </c>
-      <c r="H12" t="n">
-        <v>2.183673469387755</v>
-      </c>
-      <c r="I12" t="n">
-        <v>2.88</v>
-      </c>
-      <c r="J12" t="n">
         <v>2.88</v>
       </c>
     </row>
@@ -840,27 +688,15 @@
         <v>2.583333333333333</v>
       </c>
       <c r="C13" t="n">
-        <v>5.72</v>
+        <v>3.5</v>
       </c>
       <c r="D13" t="n">
-        <v>3.4</v>
+        <v>3.44</v>
       </c>
       <c r="E13" t="n">
-        <v>3.44</v>
+        <v>3.54</v>
       </c>
       <c r="F13" t="n">
-        <v>3.44</v>
-      </c>
-      <c r="G13" t="n">
-        <v>6.84</v>
-      </c>
-      <c r="H13" t="n">
-        <v>3.918367346938775</v>
-      </c>
-      <c r="I13" t="n">
-        <v>4.44</v>
-      </c>
-      <c r="J13" t="n">
         <v>4.44</v>
       </c>
     </row>
@@ -872,27 +708,15 @@
         <v>4.888888888888889</v>
       </c>
       <c r="C14" t="n">
-        <v>6.127659574468085</v>
+        <v>7</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>4.9375</v>
       </c>
       <c r="E14" t="n">
-        <v>4.9375</v>
+        <v>4.319148936170213</v>
       </c>
       <c r="F14" t="n">
-        <v>4.9375</v>
-      </c>
-      <c r="G14" t="n">
-        <v>6.541666666666667</v>
-      </c>
-      <c r="H14" t="n">
-        <v>4.74468085106383</v>
-      </c>
-      <c r="I14" t="n">
-        <v>3.765957446808511</v>
-      </c>
-      <c r="J14" t="n">
         <v>3.765957446808511</v>
       </c>
     </row>
@@ -904,27 +728,15 @@
         <v>3.785714285714286</v>
       </c>
       <c r="C15" t="n">
-        <v>8</v>
+        <v>4.555555555555555</v>
       </c>
       <c r="D15" t="n">
-        <v>5.170212765957447</v>
+        <v>3.608695652173913</v>
       </c>
       <c r="E15" t="n">
-        <v>3.608695652173913</v>
+        <v>9.088888888888889</v>
       </c>
       <c r="F15" t="n">
-        <v>3.608695652173913</v>
-      </c>
-      <c r="G15" t="n">
-        <v>10.97727272727273</v>
-      </c>
-      <c r="H15" t="n">
-        <v>13.51111111111111</v>
-      </c>
-      <c r="I15" t="n">
-        <v>6.642857142857143</v>
-      </c>
-      <c r="J15" t="n">
         <v>6.642857142857143</v>
       </c>
     </row>
@@ -936,27 +748,15 @@
         <v>5.694444444444445</v>
       </c>
       <c r="C16" t="n">
-        <v>6.146341463414634</v>
+        <v>4.463414634146342</v>
       </c>
       <c r="D16" t="n">
-        <v>3.853658536585366</v>
+        <v>5.8</v>
       </c>
       <c r="E16" t="n">
-        <v>5.8</v>
+        <v>8.512195121951219</v>
       </c>
       <c r="F16" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="G16" t="n">
-        <v>13.87804878048781</v>
-      </c>
-      <c r="H16" t="n">
-        <v>12</v>
-      </c>
-      <c r="I16" t="n">
-        <v>11.1025641025641</v>
-      </c>
-      <c r="J16" t="n">
         <v>11.1025641025641</v>
       </c>
     </row>
@@ -968,27 +768,15 @@
         <v>4.576923076923077</v>
       </c>
       <c r="C17" t="n">
-        <v>10.78378378378378</v>
+        <v>11.2051282051282</v>
       </c>
       <c r="D17" t="n">
-        <v>9.297297297297296</v>
+        <v>10.41025641025641</v>
       </c>
       <c r="E17" t="n">
-        <v>10.41025641025641</v>
+        <v>13</v>
       </c>
       <c r="F17" t="n">
-        <v>10.41025641025641</v>
-      </c>
-      <c r="G17" t="n">
-        <v>21.24242424242424</v>
-      </c>
-      <c r="H17" t="n">
-        <v>16.33333333333333</v>
-      </c>
-      <c r="I17" t="n">
-        <v>13.46666666666667</v>
-      </c>
-      <c r="J17" t="n">
         <v>13.46666666666667</v>
       </c>
     </row>
@@ -1000,27 +788,15 @@
         <v>5.882352941176471</v>
       </c>
       <c r="C18" t="n">
-        <v>17.93103448275862</v>
+        <v>8.857142857142858</v>
       </c>
       <c r="D18" t="n">
-        <v>9.96551724137931</v>
+        <v>14.06896551724138</v>
       </c>
       <c r="E18" t="n">
-        <v>14.06896551724138</v>
+        <v>22.125</v>
       </c>
       <c r="F18" t="n">
-        <v>14.06896551724138</v>
-      </c>
-      <c r="G18" t="n">
-        <v>24.6</v>
-      </c>
-      <c r="H18" t="n">
-        <v>26.32</v>
-      </c>
-      <c r="I18" t="n">
-        <v>16.65217391304348</v>
-      </c>
-      <c r="J18" t="n">
         <v>16.65217391304348</v>
       </c>
     </row>
@@ -1032,27 +808,15 @@
         <v>7.222222222222222</v>
       </c>
       <c r="C19" t="n">
-        <v>19.82352941176471</v>
+        <v>16.36842105263158</v>
       </c>
       <c r="D19" t="n">
-        <v>20.22727272727273</v>
+        <v>20.55</v>
       </c>
       <c r="E19" t="n">
-        <v>20.55</v>
+        <v>20.85714285714286</v>
       </c>
       <c r="F19" t="n">
-        <v>20.55</v>
-      </c>
-      <c r="G19" t="n">
-        <v>20.18181818181818</v>
-      </c>
-      <c r="H19" t="n">
-        <v>21.33333333333333</v>
-      </c>
-      <c r="I19" t="n">
-        <v>18.91666666666667</v>
-      </c>
-      <c r="J19" t="n">
         <v>18.91666666666667</v>
       </c>
     </row>
@@ -1064,27 +828,15 @@
         <v>9.25</v>
       </c>
       <c r="C20" t="n">
-        <v>24.33333333333333</v>
+        <v>11.6</v>
       </c>
       <c r="D20" t="n">
-        <v>13.2</v>
+        <v>13.8</v>
       </c>
       <c r="E20" t="n">
-        <v>13.8</v>
+        <v>18.71428571428572</v>
       </c>
       <c r="F20" t="n">
-        <v>13.8</v>
-      </c>
-      <c r="G20" t="n">
-        <v>30.25</v>
-      </c>
-      <c r="H20" t="n">
-        <v>20.66666666666667</v>
-      </c>
-      <c r="I20" t="n">
-        <v>46.28571428571428</v>
-      </c>
-      <c r="J20" t="n">
         <v>46.28571428571428</v>
       </c>
     </row>
@@ -1096,27 +848,15 @@
         <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D21" t="n">
-        <v>22.2</v>
+        <v>29.25</v>
       </c>
       <c r="E21" t="n">
-        <v>29.25</v>
+        <v>28</v>
       </c>
       <c r="F21" t="n">
-        <v>29.25</v>
-      </c>
-      <c r="G21" t="n">
-        <v>56</v>
-      </c>
-      <c r="H21" t="n">
-        <v>30.5</v>
-      </c>
-      <c r="I21" t="n">
-        <v>47</v>
-      </c>
-      <c r="J21" t="n">
         <v>47</v>
       </c>
     </row>

</xml_diff>